<commit_message>
Started on the economy; tinkered on the front
</commit_message>
<xml_diff>
--- a/Sheets/Book1.xlsx
+++ b/Sheets/Book1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\source\repos\RiskGame.API\Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3339B9F4-C95B-4B58-AD64-4E10F9554948}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8CBC45-2E93-41EB-975E-6140BB228F33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{06EB2E3F-A283-4A25-8E9C-4EB23C23B22E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{06EB2E3F-A283-4A25-8E9C-4EB23C23B22E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Income" sheetId="2" r:id="rId2"/>
+    <sheet name="Leverage" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>red</t>
   </si>
@@ -229,7 +230,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$E$1</c:f>
+              <c:f>Income!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -262,7 +263,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$D$2:$D$101</c:f>
+              <c:f>Income!$D$2:$D$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -571,7 +572,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$E$2:$E$101</c:f>
+              <c:f>Income!$E$2:$E$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -1127,7 +1128,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$F$1</c:f>
+              <c:f>Income!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1160,7 +1161,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$D$2:$D$101</c:f>
+              <c:f>Income!$D$2:$D$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -1469,7 +1470,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$F$2:$F$101</c:f>
+              <c:f>Income!$F$2:$F$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -1967,6 +1968,1800 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Leverage!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Leverage!$D$2:$D$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0999999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9000000000000006</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.0000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2000000000000006</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.4000000000000008</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5000000000000009</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.7000000000000011</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8000000000000012</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.9000000000000012</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.0000000000000013</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.1000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.2000000000000015</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.3000000000000016</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.4000000000000017</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.5000000000000018</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.6000000000000019</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.9000000000000021</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.0000000000000018</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.1000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.2000000000000011</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.7999999999999989</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.8999999999999986</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.9999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.0999999999999979</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.1999999999999975</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.2999999999999972</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.3999999999999968</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.4999999999999964</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.5999999999999961</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.6999999999999957</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.7999999999999954</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.899999999999995</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5.9999999999999947</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.0999999999999943</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.199999999999994</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.2999999999999936</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.3999999999999932</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.4999999999999929</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.5999999999999925</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6.6999999999999922</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.7999999999999918</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.8999999999999915</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>6.9999999999999911</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7.0999999999999908</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7.1999999999999904</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.2999999999999901</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.3999999999999897</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.4999999999999893</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.599999999999989</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7.6999999999999886</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7.7999999999999883</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>7.8999999999999879</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>7.9999999999999876</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>8.0999999999999872</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8.1999999999999869</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>8.2999999999999865</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>8.3999999999999861</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8.4999999999999858</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>8.5999999999999854</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>8.6999999999999851</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8.7999999999999847</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>8.8999999999999844</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>8.999999999999984</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>9.0999999999999837</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>9.1999999999999833</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9.2999999999999829</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9.3999999999999826</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9.4999999999999822</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9.5999999999999819</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9.6999999999999815</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9.7999999999999812</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>9.8999999999999808</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Leverage!$E$2:$E$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.20202020202020202</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2040816326530612</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2061855670103093</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.20833333333333334</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.21052631578947367</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.21276595744680851</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.21505376344086019</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.21739130434782611</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.21978021978021978</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.22222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.2247191011235955</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.22727272727272727</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.22988505747126439</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.23255813953488372</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.23529411764705882</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.23809523809523808</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.24096385542168677</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.24390243902439027</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.24691358024691359</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.25316455696202533</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.25641025641025644</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.25974025974025977</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.26315789473684209</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.26666666666666672</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.27027027027027034</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.27397260273972607</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.27777777777777779</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.28169014084507049</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.28571428571428581</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.28985507246376818</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.29411764705882359</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.29850746268656725</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.30303030303030315</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.30769230769230776</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.31250000000000006</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.31746031746031755</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.32258064516129042</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.32786885245901654</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.33333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.33898305084745772</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.34482758620689663</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.35087719298245618</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.35714285714285715</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.36363636363636365</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.37037037037037035</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.37735849056603771</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.38461538461538453</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.39215686274509792</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.39999999999999986</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.40816326530612229</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.41666666666666646</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.42553191489361675</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.43478260869565188</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.44444444444444409</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.45454545454545414</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.46511627906976699</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.47619047619047566</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.48780487804877992</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.49999999999999933</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.51282051282051211</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.5263157894736834</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.54054054054053957</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.55555555555555447</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.57142857142857029</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.58823529411764575</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.60606060606060463</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.62499999999999845</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.64516129032257885</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.66666666666666474</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.68965517241379093</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.71428571428571186</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.74074074074073804</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.76923076923076616</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.7999999999999966</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.83333333333332948</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.8695652173913001</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.90909090909090429</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.95238095238094689</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.99999999999999378</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1.0526315789473613</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1.1111111111111029</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1.1764705882352848</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.2499999999999891</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1.3333333333333206</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1.4285714285714137</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1.5384615384615208</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1.6666666666666454</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1.8181818181817924</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1.999999999999968</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2.2222222222221819</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2.499999999999948</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2.8571428571427875</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3.3333333333332367</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3.9999999999998579</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>4.9999999999997735</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>6.6666666666662557</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9.9999999999990585</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>19.999999999996163</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-37CD-4E01-9F41-619F2FA331EE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="688490144"/>
+        <c:axId val="688490472"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="688490144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="688490472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="688490472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="688490144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Leverage!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>d1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Leverage!$D$2:$D$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99999999999999989</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0999999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9000000000000006</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.0000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.1000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2000000000000006</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.4000000000000008</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5000000000000009</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.7000000000000011</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8000000000000012</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.9000000000000012</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.0000000000000013</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.1000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.2000000000000015</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.3000000000000016</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.4000000000000017</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.5000000000000018</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.6000000000000019</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.9000000000000021</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.0000000000000018</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.1000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.2000000000000011</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.7999999999999989</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.8999999999999986</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.9999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.0999999999999979</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.1999999999999975</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.2999999999999972</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.3999999999999968</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.4999999999999964</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.5999999999999961</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.6999999999999957</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.7999999999999954</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.899999999999995</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5.9999999999999947</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.0999999999999943</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.199999999999994</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.2999999999999936</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.3999999999999932</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.4999999999999929</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.5999999999999925</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6.6999999999999922</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.7999999999999918</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.8999999999999915</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>6.9999999999999911</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7.0999999999999908</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7.1999999999999904</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.2999999999999901</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.3999999999999897</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.4999999999999893</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.599999999999989</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7.6999999999999886</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7.7999999999999883</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>7.8999999999999879</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>7.9999999999999876</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>8.0999999999999872</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8.1999999999999869</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>8.2999999999999865</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>8.3999999999999861</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8.4999999999999858</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>8.5999999999999854</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>8.6999999999999851</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8.7999999999999847</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>8.8999999999999844</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>8.999999999999984</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>9.0999999999999837</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>9.1999999999999833</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>9.2999999999999829</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>9.3999999999999826</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>9.4999999999999822</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>9.5999999999999819</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>9.6999999999999815</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>9.7999999999999812</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>9.8999999999999808</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Leverage!$F$2:$F$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="1">
+                  <c:v>1.0101010101010027E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0204081632652965E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0309278350515661E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.041666666666663E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0526315789473583E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0638297872340489E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0752688172042887E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0869565217391521E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0989010989010872E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1111111111111072E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1235955056179803E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1363636363636359E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.149425287356336E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1627906976744064E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.1764705882352941E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.1904761904761862E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.2048192771084505E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2195121951219494E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.2345679012345644E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.2499999999999942E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.2658227848101333E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.2820512820512883E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.2987012987012979E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.3157894736841928E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.3333333333333586E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.351351351351358E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.3698630136986186E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.3888888888888784E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.4084507042253724E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.4285714285714375E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.4492753623188298E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.4705882352941171E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.492537313432842E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.5151515151515265E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.5384615384615224E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.5624999999999941E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.587301587301599E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.612903225806454E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.6393442622950938E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.666666666666651E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.6949152542372888E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.7241379310344772E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.7543859649122681E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.7857142857142776E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.8181818181818188E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.8518518518518434E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.8867924528301869E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.9230769230769069E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.9607843137254836E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.9999999999999934E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.0408163265306097E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.0833333333333228E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.1276595744680691E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.1739130434782587E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.2222222222222081E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.2727272727272641E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2.3255813953488289E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.3809523809523669E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.4390243902438966E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.4999999999999824E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.5641025641025585E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.6315789473684063E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.7027027027026758E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.7777777777777613E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2.8571428571428525E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.9411764705882113E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.0303030303030176E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.1249999999999861E-2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.2258064516128726E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.3333333333333222E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3.4482758620689377E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.5714285714285463E-2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3.7037037037036771E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.8461538461538117E-2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3.999999999999973E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4.1666666666666276E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4.3478260869564946E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>4.5454545454545033E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4.761904761904711E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4.9999999999999531E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>5.2631578947367801E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>5.5555555555554983E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>5.8823529411764129E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>6.249999999999914E-2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>6.6666666666665764E-2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>7.1428571428570523E-2</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>7.6923076923075734E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8.3333333333331969E-2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>9.0909090909089316E-2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9.9999999999998035E-2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.11111111111110872</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.12499999999999703</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.14285714285713874</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.16666666666666127</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.19999999999999216</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.24999999999998779</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.33333333333331155</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.49999999999995126</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.9999999999998046</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EC2C-4E89-AAE6-AAFFF46E8275}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="450304664"/>
+        <c:axId val="450302040"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="450304664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="450302040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="450302040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="450304664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2047,6 +3842,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2564,6 +4439,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3136,6 +6043,83 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB6F9E50-80A5-4ED6-80F1-E6001DEBFB23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E81FB76-26CF-4121-BA98-162A0C32F12A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02DF17F2-7C18-45BD-991B-FE2F608ED954}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3455,8 +6439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B609C2-EE89-4843-8472-037D68741DF9}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3512,11 +6496,11 @@
       </c>
       <c r="B4">
         <f ca="1">RANDBETWEEN(0,75)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(-100,100)</f>
-        <v>-2</v>
+        <v>93</v>
       </c>
       <c r="D4">
         <f ca="1">FLOOR(5.2/(1+EXP(0.4*(RANDBETWEEN(0,100)-30))),1)</f>
@@ -3524,11 +6508,11 @@
       </c>
       <c r="E4">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="F4">
         <f ca="1">RANDBETWEEN(-100,100)</f>
-        <v>37</v>
+        <v>-61</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3537,23 +6521,23 @@
       </c>
       <c r="B5">
         <f t="shared" ref="B5:B9" ca="1" si="0">RANDBETWEEN(0,75)</f>
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:C9" ca="1" si="1">RANDBETWEEN(-100,100)</f>
-        <v>95</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D9" ca="1" si="2">FLOOR(5.2/(1+EXP(0.4*(RANDBETWEEN(0,100)-30))),1)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <f t="shared" ref="E5:E9" ca="1" si="3">RANDBETWEEN(0,100)</f>
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F5">
         <f t="shared" ref="F5:F9" ca="1" si="4">RANDBETWEEN(-100,100)</f>
-        <v>-72</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3562,11 +6546,11 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>-88</v>
+        <v>-96</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="2"/>
@@ -3574,11 +6558,11 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="3"/>
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="4"/>
-        <v>41</v>
+        <v>-37</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3587,11 +6571,11 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>-29</v>
+        <v>-24</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="2"/>
@@ -3599,11 +6583,11 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="3"/>
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="4"/>
-        <v>-55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3612,23 +6596,23 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="3"/>
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="4"/>
-        <v>-83</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3637,11 +6621,11 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>-34</v>
+        <v>-24</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="2"/>
@@ -3649,11 +6633,11 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="4"/>
-        <v>11</v>
+        <v>-87</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3690,7 +6674,7 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5139,4 +8123,1454 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D109173-DB42-4968-B036-C5B76C1D5038}">
+  <dimension ref="A1:F101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <f>$B$1</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>$B$4/(D2-$B$5)</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <f t="shared" ref="D3:D67" si="0">($B$2-$B$1)/100+D2</f>
+        <v>0.1</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E66" si="1">$B$4/(D3-$B$5)</f>
+        <v>0.20202020202020202</v>
+      </c>
+      <c r="F3">
+        <f>(E3-E2)/E2</f>
+        <v>1.0101010101010027E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>-2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>0.2040816326530612</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F67" si="2">(E4-E3)/E3</f>
+        <v>1.0204081632652965E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>0.2061855670103093</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>1.0309278350515661E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>0.21052631578947367</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>1.0526315789473583E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>0.21276595744680851</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>1.0638297872340489E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>0.21505376344086019</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>1.0752688172042887E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>0.21739130434782611</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>1.0869565217391521E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0.21978021978021978</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>1.0989010989010872E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>1.1111111111111072E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>0.2247191011235955</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>1.1235955056179803E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>0.22727272727272727</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>1.1363636363636359E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>0.22988505747126439</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>1.149425287356336E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>0.23255813953488372</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>1.1627906976744064E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>1.5000000000000002</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>0.23529411764705882</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>1.1764705882352941E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>1.6000000000000003</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>0.23809523809523808</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>1.1904761904761862E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>1.7000000000000004</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>0.24096385542168677</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>1.2048192771084505E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>1.8000000000000005</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>0.24390243902439027</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>1.2195121951219494E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>1.9000000000000006</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>0.24691358024691359</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>1.2345679012345644E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>2.0000000000000004</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>1.2499999999999942E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>2.1000000000000005</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>0.25316455696202533</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="2"/>
+        <v>1.2658227848101333E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>2.2000000000000006</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>0.25641025641025644</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>1.2820512820512883E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>2.3000000000000007</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>0.25974025974025977</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>1.2987012987012979E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>2.4000000000000008</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>0.26315789473684209</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="2"/>
+        <v>1.3157894736841928E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000009</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>0.26666666666666672</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="2"/>
+        <v>1.3333333333333586E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>2.600000000000001</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>0.27027027027027034</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="2"/>
+        <v>1.351351351351358E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>2.7000000000000011</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>0.27397260273972607</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="2"/>
+        <v>1.3698630136986186E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>2.8000000000000012</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="2"/>
+        <v>1.3888888888888784E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>2.9000000000000012</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>0.28169014084507049</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="2"/>
+        <v>1.4084507042253724E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>3.0000000000000013</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>0.28571428571428581</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="2"/>
+        <v>1.4285714285714375E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>3.1000000000000014</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>0.28985507246376818</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="2"/>
+        <v>1.4492753623188298E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>3.2000000000000015</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>0.29411764705882359</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="2"/>
+        <v>1.4705882352941171E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>3.3000000000000016</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>0.29850746268656725</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="2"/>
+        <v>1.492537313432842E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>3.4000000000000017</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>0.30303030303030315</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="2"/>
+        <v>1.5151515151515265E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>3.5000000000000018</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>0.30769230769230776</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="2"/>
+        <v>1.5384615384615224E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>3.6000000000000019</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>0.31250000000000006</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="2"/>
+        <v>1.5624999999999941E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>3.700000000000002</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>0.31746031746031755</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="2"/>
+        <v>1.587301587301599E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>3.800000000000002</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="1"/>
+        <v>0.32258064516129042</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="2"/>
+        <v>1.612903225806454E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>3.9000000000000021</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="1"/>
+        <v>0.32786885245901654</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="2"/>
+        <v>1.6393442622950938E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000018</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333343</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="2"/>
+        <v>1.666666666666651E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>4.1000000000000014</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>0.33898305084745772</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="2"/>
+        <v>1.6949152542372888E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>4.2000000000000011</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>0.34482758620689663</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="2"/>
+        <v>1.7241379310344772E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>4.3000000000000007</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>0.35087719298245618</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="2"/>
+        <v>1.7543859649122681E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="2"/>
+        <v>1.7857142857142776E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="1"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="2"/>
+        <v>1.8181818181818188E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="1"/>
+        <v>0.37037037037037035</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="2"/>
+        <v>1.8518518518518434E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>4.6999999999999993</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="1"/>
+        <v>0.37735849056603771</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="2"/>
+        <v>1.8867924528301869E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>4.7999999999999989</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="1"/>
+        <v>0.38461538461538453</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="2"/>
+        <v>1.9230769230769069E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>4.8999999999999986</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="1"/>
+        <v>0.39215686274509792</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="2"/>
+        <v>1.9607843137254836E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>4.9999999999999982</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="1"/>
+        <v>0.39999999999999986</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="2"/>
+        <v>1.9999999999999934E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>5.0999999999999979</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="1"/>
+        <v>0.40816326530612229</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="2"/>
+        <v>2.0408163265306097E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>5.1999999999999975</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="1"/>
+        <v>0.41666666666666646</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="2"/>
+        <v>2.0833333333333228E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>5.2999999999999972</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="1"/>
+        <v>0.42553191489361675</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="2"/>
+        <v>2.1276595744680691E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>5.3999999999999968</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="1"/>
+        <v>0.43478260869565188</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="2"/>
+        <v>2.1739130434782587E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>5.4999999999999964</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="1"/>
+        <v>0.44444444444444409</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="2"/>
+        <v>2.2222222222222081E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>5.5999999999999961</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="1"/>
+        <v>0.45454545454545414</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="2"/>
+        <v>2.2727272727272641E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>5.6999999999999957</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="1"/>
+        <v>0.46511627906976699</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="2"/>
+        <v>2.3255813953488289E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>5.7999999999999954</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="1"/>
+        <v>0.47619047619047566</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="2"/>
+        <v>2.3809523809523669E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>5.899999999999995</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="1"/>
+        <v>0.48780487804877992</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="2"/>
+        <v>2.4390243902438966E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>5.9999999999999947</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="1"/>
+        <v>0.49999999999999933</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="2"/>
+        <v>2.4999999999999824E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>6.0999999999999943</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="1"/>
+        <v>0.51282051282051211</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="2"/>
+        <v>2.5641025641025585E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>6.199999999999994</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="1"/>
+        <v>0.5263157894736834</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="2"/>
+        <v>2.6315789473684063E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>6.2999999999999936</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="1"/>
+        <v>0.54054054054053957</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="2"/>
+        <v>2.7027027027026758E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>6.3999999999999932</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="1"/>
+        <v>0.55555555555555447</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="2"/>
+        <v>2.7777777777777613E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <f t="shared" si="0"/>
+        <v>6.4999999999999929</v>
+      </c>
+      <c r="E67">
+        <f t="shared" ref="E67:E101" si="3">$B$4/(D67-$B$5)</f>
+        <v>0.57142857142857029</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="2"/>
+        <v>2.8571428571428525E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <f t="shared" ref="D68:D101" si="4">($B$2-$B$1)/100+D67</f>
+        <v>6.5999999999999925</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="3"/>
+        <v>0.58823529411764575</v>
+      </c>
+      <c r="F68">
+        <f t="shared" ref="F68:F101" si="5">(E68-E67)/E67</f>
+        <v>2.9411764705882113E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <f t="shared" si="4"/>
+        <v>6.6999999999999922</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="3"/>
+        <v>0.60606060606060463</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="5"/>
+        <v>3.0303030303030176E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <f t="shared" si="4"/>
+        <v>6.7999999999999918</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="3"/>
+        <v>0.62499999999999845</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="5"/>
+        <v>3.1249999999999861E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <f t="shared" si="4"/>
+        <v>6.8999999999999915</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="3"/>
+        <v>0.64516129032257885</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="5"/>
+        <v>3.2258064516128726E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <f t="shared" si="4"/>
+        <v>6.9999999999999911</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666474</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333222E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <f t="shared" si="4"/>
+        <v>7.0999999999999908</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="3"/>
+        <v>0.68965517241379093</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="5"/>
+        <v>3.4482758620689377E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <f t="shared" si="4"/>
+        <v>7.1999999999999904</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="3"/>
+        <v>0.71428571428571186</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="5"/>
+        <v>3.5714285714285463E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <f t="shared" si="4"/>
+        <v>7.2999999999999901</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="3"/>
+        <v>0.74074074074073804</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="5"/>
+        <v>3.7037037037036771E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <f t="shared" si="4"/>
+        <v>7.3999999999999897</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="3"/>
+        <v>0.76923076923076616</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="5"/>
+        <v>3.8461538461538117E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <f t="shared" si="4"/>
+        <v>7.4999999999999893</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="3"/>
+        <v>0.7999999999999966</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="5"/>
+        <v>3.999999999999973E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <f t="shared" si="4"/>
+        <v>7.599999999999989</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="3"/>
+        <v>0.83333333333332948</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="5"/>
+        <v>4.1666666666666276E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <f t="shared" si="4"/>
+        <v>7.6999999999999886</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="3"/>
+        <v>0.8695652173913001</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="5"/>
+        <v>4.3478260869564946E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <f t="shared" si="4"/>
+        <v>7.7999999999999883</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="3"/>
+        <v>0.90909090909090429</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="5"/>
+        <v>4.5454545454545033E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D81">
+        <f t="shared" si="4"/>
+        <v>7.8999999999999879</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="3"/>
+        <v>0.95238095238094689</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="5"/>
+        <v>4.761904761904711E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D82">
+        <f t="shared" si="4"/>
+        <v>7.9999999999999876</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="3"/>
+        <v>0.99999999999999378</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="5"/>
+        <v>4.9999999999999531E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D83">
+        <f t="shared" si="4"/>
+        <v>8.0999999999999872</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="3"/>
+        <v>1.0526315789473613</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="5"/>
+        <v>5.2631578947367801E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D84">
+        <f t="shared" si="4"/>
+        <v>8.1999999999999869</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="3"/>
+        <v>1.1111111111111029</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="5"/>
+        <v>5.5555555555554983E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D85">
+        <f t="shared" si="4"/>
+        <v>8.2999999999999865</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="3"/>
+        <v>1.1764705882352848</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="5"/>
+        <v>5.8823529411764129E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D86">
+        <f t="shared" si="4"/>
+        <v>8.3999999999999861</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="3"/>
+        <v>1.2499999999999891</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="5"/>
+        <v>6.249999999999914E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D87">
+        <f t="shared" si="4"/>
+        <v>8.4999999999999858</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="3"/>
+        <v>1.3333333333333206</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="5"/>
+        <v>6.6666666666665764E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D88">
+        <f t="shared" si="4"/>
+        <v>8.5999999999999854</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="3"/>
+        <v>1.4285714285714137</v>
+      </c>
+      <c r="F88">
+        <f t="shared" si="5"/>
+        <v>7.1428571428570523E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D89">
+        <f t="shared" si="4"/>
+        <v>8.6999999999999851</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="3"/>
+        <v>1.5384615384615208</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="5"/>
+        <v>7.6923076923075734E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D90">
+        <f t="shared" si="4"/>
+        <v>8.7999999999999847</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="3"/>
+        <v>1.6666666666666454</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="5"/>
+        <v>8.3333333333331969E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D91">
+        <f t="shared" si="4"/>
+        <v>8.8999999999999844</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="3"/>
+        <v>1.8181818181817924</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="5"/>
+        <v>9.0909090909089316E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D92">
+        <f t="shared" si="4"/>
+        <v>8.999999999999984</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="3"/>
+        <v>1.999999999999968</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="5"/>
+        <v>9.9999999999998035E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D93">
+        <f t="shared" si="4"/>
+        <v>9.0999999999999837</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="3"/>
+        <v>2.2222222222221819</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="5"/>
+        <v>0.11111111111110872</v>
+      </c>
+    </row>
+    <row r="94" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D94">
+        <f t="shared" si="4"/>
+        <v>9.1999999999999833</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="3"/>
+        <v>2.499999999999948</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="5"/>
+        <v>0.12499999999999703</v>
+      </c>
+    </row>
+    <row r="95" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D95">
+        <f t="shared" si="4"/>
+        <v>9.2999999999999829</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="3"/>
+        <v>2.8571428571427875</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="5"/>
+        <v>0.14285714285713874</v>
+      </c>
+    </row>
+    <row r="96" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D96">
+        <f t="shared" si="4"/>
+        <v>9.3999999999999826</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="3"/>
+        <v>3.3333333333332367</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="5"/>
+        <v>0.16666666666666127</v>
+      </c>
+    </row>
+    <row r="97" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D97">
+        <f t="shared" si="4"/>
+        <v>9.4999999999999822</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="3"/>
+        <v>3.9999999999998579</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="5"/>
+        <v>0.19999999999999216</v>
+      </c>
+    </row>
+    <row r="98" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D98">
+        <f t="shared" si="4"/>
+        <v>9.5999999999999819</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="3"/>
+        <v>4.9999999999997735</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="5"/>
+        <v>0.24999999999998779</v>
+      </c>
+    </row>
+    <row r="99" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D99">
+        <f t="shared" si="4"/>
+        <v>9.6999999999999815</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="3"/>
+        <v>6.6666666666662557</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="5"/>
+        <v>0.33333333333331155</v>
+      </c>
+    </row>
+    <row r="100" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D100">
+        <f t="shared" si="4"/>
+        <v>9.7999999999999812</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="3"/>
+        <v>9.9999999999990585</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="5"/>
+        <v>0.49999999999995126</v>
+      </c>
+    </row>
+    <row r="101" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D101">
+        <f t="shared" si="4"/>
+        <v>9.8999999999999808</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="3"/>
+        <v>19.999999999996163</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="5"/>
+        <v>0.9999999999998046</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Worked on the game progression
</commit_message>
<xml_diff>
--- a/Sheets/Book1.xlsx
+++ b/Sheets/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\source\repos\RiskGame.API\Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8CBC45-2E93-41EB-975E-6140BB228F33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6459D2-2E86-450B-859D-4583EAB55FCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{06EB2E3F-A283-4A25-8E9C-4EB23C23B22E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{06EB2E3F-A283-4A25-8E9C-4EB23C23B22E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>red</t>
   </si>
@@ -2867,901 +2867,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Leverage!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>d1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Leverage!$D$2:$D$101</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.30000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.79999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.89999999999999991</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.99999999999999989</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.0999999999999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.4000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.5000000000000002</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.6000000000000003</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.7000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.8000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.9000000000000006</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.0000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2.1000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2.2000000000000006</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2.3000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2.4000000000000008</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2.5000000000000009</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2.600000000000001</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2.7000000000000011</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2.8000000000000012</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2.9000000000000012</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3.0000000000000013</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>3.1000000000000014</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>3.2000000000000015</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>3.3000000000000016</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>3.4000000000000017</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>3.5000000000000018</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>3.6000000000000019</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>3.700000000000002</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>3.800000000000002</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>3.9000000000000021</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>4.0000000000000018</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>4.1000000000000014</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>4.2000000000000011</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>4.3000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>4.4000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>4.5999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>4.6999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>4.7999999999999989</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>4.8999999999999986</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>4.9999999999999982</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>5.0999999999999979</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>5.1999999999999975</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>5.2999999999999972</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>5.3999999999999968</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>5.4999999999999964</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>5.5999999999999961</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>5.6999999999999957</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>5.7999999999999954</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5.899999999999995</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>5.9999999999999947</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>6.0999999999999943</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>6.199999999999994</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>6.2999999999999936</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>6.3999999999999932</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>6.4999999999999929</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>6.5999999999999925</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>6.6999999999999922</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>6.7999999999999918</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>6.8999999999999915</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>6.9999999999999911</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>7.0999999999999908</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>7.1999999999999904</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>7.2999999999999901</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>7.3999999999999897</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>7.4999999999999893</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>7.599999999999989</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>7.6999999999999886</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>7.7999999999999883</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>7.8999999999999879</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>7.9999999999999876</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>8.0999999999999872</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>8.1999999999999869</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>8.2999999999999865</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>8.3999999999999861</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>8.4999999999999858</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>8.5999999999999854</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>8.6999999999999851</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>8.7999999999999847</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>8.8999999999999844</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>8.999999999999984</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>9.0999999999999837</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>9.1999999999999833</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>9.2999999999999829</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>9.3999999999999826</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>9.4999999999999822</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>9.5999999999999819</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>9.6999999999999815</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>9.7999999999999812</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>9.8999999999999808</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Leverage!$F$2:$F$101</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
-                <c:pt idx="1">
-                  <c:v>1.0101010101010027E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0204081632652965E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0309278350515661E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.041666666666663E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0526315789473583E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0638297872340489E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0752688172042887E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.0869565217391521E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0989010989010872E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.1111111111111072E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.1235955056179803E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.1363636363636359E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.149425287356336E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.1627906976744064E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.1764705882352941E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.1904761904761862E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.2048192771084505E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.2195121951219494E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.2345679012345644E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.2499999999999942E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.2658227848101333E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.2820512820512883E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.2987012987012979E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.3157894736841928E-2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1.3333333333333586E-2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1.351351351351358E-2</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1.3698630136986186E-2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1.3888888888888784E-2</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1.4084507042253724E-2</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1.4285714285714375E-2</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1.4492753623188298E-2</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>1.4705882352941171E-2</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1.492537313432842E-2</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1.5151515151515265E-2</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1.5384615384615224E-2</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1.5624999999999941E-2</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>1.587301587301599E-2</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1.612903225806454E-2</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>1.6393442622950938E-2</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>1.666666666666651E-2</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>1.6949152542372888E-2</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>1.7241379310344772E-2</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>1.7543859649122681E-2</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1.7857142857142776E-2</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>1.8181818181818188E-2</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>1.8518518518518434E-2</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>1.8867924528301869E-2</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>1.9230769230769069E-2</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>1.9607843137254836E-2</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>1.9999999999999934E-2</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>2.0408163265306097E-2</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>2.0833333333333228E-2</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>2.1276595744680691E-2</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>2.1739130434782587E-2</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>2.2222222222222081E-2</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>2.2727272727272641E-2</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>2.3255813953488289E-2</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>2.3809523809523669E-2</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>2.4390243902438966E-2</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>2.4999999999999824E-2</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>2.5641025641025585E-2</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>2.6315789473684063E-2</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>2.7027027027026758E-2</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>2.7777777777777613E-2</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>2.8571428571428525E-2</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>2.9411764705882113E-2</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>3.0303030303030176E-2</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>3.1249999999999861E-2</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>3.2258064516128726E-2</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>3.3333333333333222E-2</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>3.4482758620689377E-2</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>3.5714285714285463E-2</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>3.7037037037036771E-2</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>3.8461538461538117E-2</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>3.999999999999973E-2</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>4.1666666666666276E-2</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>4.3478260869564946E-2</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>4.5454545454545033E-2</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>4.761904761904711E-2</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>4.9999999999999531E-2</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>5.2631578947367801E-2</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>5.5555555555554983E-2</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>5.8823529411764129E-2</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>6.249999999999914E-2</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>6.6666666666665764E-2</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>7.1428571428570523E-2</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>7.6923076923075734E-2</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>8.3333333333331969E-2</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>9.0909090909089316E-2</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>9.9999999999998035E-2</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.11111111111110872</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.12499999999999703</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.14285714285713874</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.16666666666666127</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.19999999999999216</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.24999999999998779</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.33333333333331155</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>0.49999999999995126</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.9999999999998046</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EC2C-4E89-AAE6-AAFFF46E8275}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="450304664"/>
-        <c:axId val="450302040"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="450304664"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="450302040"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="450302040"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="450304664"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3882,46 +2987,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4955,522 +4020,6 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6067,16 +4616,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6096,42 +4645,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02DF17F2-7C18-45BD-991B-FE2F608ED954}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6496,11 +5009,11 @@
       </c>
       <c r="B4">
         <f ca="1">RANDBETWEEN(0,75)</f>
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(-100,100)</f>
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <f ca="1">FLOOR(5.2/(1+EXP(0.4*(RANDBETWEEN(0,100)-30))),1)</f>
@@ -6508,11 +5021,11 @@
       </c>
       <c r="E4">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="F4">
         <f ca="1">RANDBETWEEN(-100,100)</f>
-        <v>-61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -6521,11 +5034,11 @@
       </c>
       <c r="B5">
         <f t="shared" ref="B5:B9" ca="1" si="0">RANDBETWEEN(0,75)</f>
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:C9" ca="1" si="1">RANDBETWEEN(-100,100)</f>
-        <v>5</v>
+        <v>87</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D9" ca="1" si="2">FLOOR(5.2/(1+EXP(0.4*(RANDBETWEEN(0,100)-30))),1)</f>
@@ -6533,11 +5046,11 @@
       </c>
       <c r="E5">
         <f t="shared" ref="E5:E9" ca="1" si="3">RANDBETWEEN(0,100)</f>
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="F5">
         <f t="shared" ref="F5:F9" ca="1" si="4">RANDBETWEEN(-100,100)</f>
-        <v>-5</v>
+        <v>-31</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -6546,23 +5059,23 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>-96</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="3"/>
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="4"/>
-        <v>-37</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -6571,11 +5084,11 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>-24</v>
+        <v>-95</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="2"/>
@@ -6583,11 +5096,11 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="3"/>
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="4"/>
-        <v>62</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -6596,23 +5109,23 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="3"/>
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="4"/>
-        <v>99</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -6621,11 +5134,11 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>-24</v>
+        <v>-52</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="2"/>
@@ -6633,11 +5146,11 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="4"/>
-        <v>-87</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -6673,8 +5186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F033D2C1-474E-472E-8C88-41BDEFE5D9CE}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8127,10 +6640,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D109173-DB42-4968-B036-C5B76C1D5038}">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8138,7 +6651,7 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -8151,11 +6664,8 @@
       <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -8171,7 +6681,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D3">
         <f t="shared" ref="D3:D67" si="0">($B$2-$B$1)/100+D2</f>
         <v>0.1</v>
@@ -8180,12 +6690,8 @@
         <f t="shared" ref="E3:E66" si="1">$B$4/(D3-$B$5)</f>
         <v>0.20202020202020202</v>
       </c>
-      <c r="F3">
-        <f>(E3-E2)/E2</f>
-        <v>1.0101010101010027E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -8200,12 +6706,8 @@
         <f t="shared" si="1"/>
         <v>0.2040816326530612</v>
       </c>
-      <c r="F4">
-        <f t="shared" ref="F4:F67" si="2">(E4-E3)/E3</f>
-        <v>1.0204081632652965E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -8220,12 +6722,8 @@
         <f t="shared" si="1"/>
         <v>0.2061855670103093</v>
       </c>
-      <c r="F5">
-        <f t="shared" si="2"/>
-        <v>1.0309278350515661E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D6">
         <f t="shared" si="0"/>
         <v>0.4</v>
@@ -8234,12 +6732,8 @@
         <f t="shared" si="1"/>
         <v>0.20833333333333334</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="2"/>
-        <v>1.041666666666663E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D7">
         <f t="shared" si="0"/>
         <v>0.5</v>
@@ -8248,12 +6742,8 @@
         <f t="shared" si="1"/>
         <v>0.21052631578947367</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="2"/>
-        <v>1.0526315789473583E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D8">
         <f t="shared" si="0"/>
         <v>0.6</v>
@@ -8262,12 +6752,8 @@
         <f t="shared" si="1"/>
         <v>0.21276595744680851</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="2"/>
-        <v>1.0638297872340489E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9">
         <f t="shared" si="0"/>
         <v>0.7</v>
@@ -8276,12 +6762,8 @@
         <f t="shared" si="1"/>
         <v>0.21505376344086019</v>
       </c>
-      <c r="F9">
-        <f t="shared" si="2"/>
-        <v>1.0752688172042887E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D10">
         <f t="shared" si="0"/>
         <v>0.79999999999999993</v>
@@ -8290,12 +6772,8 @@
         <f t="shared" si="1"/>
         <v>0.21739130434782611</v>
       </c>
-      <c r="F10">
-        <f t="shared" si="2"/>
-        <v>1.0869565217391521E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D11">
         <f t="shared" si="0"/>
         <v>0.89999999999999991</v>
@@ -8304,12 +6782,8 @@
         <f t="shared" si="1"/>
         <v>0.21978021978021978</v>
       </c>
-      <c r="F11">
-        <f t="shared" si="2"/>
-        <v>1.0989010989010872E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D12">
         <f t="shared" si="0"/>
         <v>0.99999999999999989</v>
@@ -8318,12 +6792,8 @@
         <f t="shared" si="1"/>
         <v>0.22222222222222221</v>
       </c>
-      <c r="F12">
-        <f t="shared" si="2"/>
-        <v>1.1111111111111072E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D13">
         <f t="shared" si="0"/>
         <v>1.0999999999999999</v>
@@ -8332,12 +6802,8 @@
         <f t="shared" si="1"/>
         <v>0.2247191011235955</v>
       </c>
-      <c r="F13">
-        <f t="shared" si="2"/>
-        <v>1.1235955056179803E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D14">
         <f t="shared" si="0"/>
         <v>1.2</v>
@@ -8346,12 +6812,8 @@
         <f t="shared" si="1"/>
         <v>0.22727272727272727</v>
       </c>
-      <c r="F14">
-        <f t="shared" si="2"/>
-        <v>1.1363636363636359E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15">
         <f t="shared" si="0"/>
         <v>1.3</v>
@@ -8360,12 +6822,8 @@
         <f t="shared" si="1"/>
         <v>0.22988505747126439</v>
       </c>
-      <c r="F15">
-        <f t="shared" si="2"/>
-        <v>1.149425287356336E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D16">
         <f t="shared" si="0"/>
         <v>1.4000000000000001</v>
@@ -8374,12 +6832,8 @@
         <f t="shared" si="1"/>
         <v>0.23255813953488372</v>
       </c>
-      <c r="F16">
-        <f t="shared" si="2"/>
-        <v>1.1627906976744064E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17">
         <f t="shared" si="0"/>
         <v>1.5000000000000002</v>
@@ -8388,12 +6842,8 @@
         <f t="shared" si="1"/>
         <v>0.23529411764705882</v>
       </c>
-      <c r="F17">
-        <f t="shared" si="2"/>
-        <v>1.1764705882352941E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18">
         <f t="shared" si="0"/>
         <v>1.6000000000000003</v>
@@ -8402,12 +6852,8 @@
         <f t="shared" si="1"/>
         <v>0.23809523809523808</v>
       </c>
-      <c r="F18">
-        <f t="shared" si="2"/>
-        <v>1.1904761904761862E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D19">
         <f t="shared" si="0"/>
         <v>1.7000000000000004</v>
@@ -8416,12 +6862,8 @@
         <f t="shared" si="1"/>
         <v>0.24096385542168677</v>
       </c>
-      <c r="F19">
-        <f t="shared" si="2"/>
-        <v>1.2048192771084505E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D20">
         <f t="shared" si="0"/>
         <v>1.8000000000000005</v>
@@ -8430,12 +6872,8 @@
         <f t="shared" si="1"/>
         <v>0.24390243902439027</v>
       </c>
-      <c r="F20">
-        <f t="shared" si="2"/>
-        <v>1.2195121951219494E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D21">
         <f t="shared" si="0"/>
         <v>1.9000000000000006</v>
@@ -8444,12 +6882,8 @@
         <f t="shared" si="1"/>
         <v>0.24691358024691359</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="2"/>
-        <v>1.2345679012345644E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D22">
         <f t="shared" si="0"/>
         <v>2.0000000000000004</v>
@@ -8458,12 +6892,8 @@
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="F22">
-        <f t="shared" si="2"/>
-        <v>1.2499999999999942E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D23">
         <f t="shared" si="0"/>
         <v>2.1000000000000005</v>
@@ -8472,12 +6902,8 @@
         <f t="shared" si="1"/>
         <v>0.25316455696202533</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="2"/>
-        <v>1.2658227848101333E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D24">
         <f t="shared" si="0"/>
         <v>2.2000000000000006</v>
@@ -8486,12 +6912,8 @@
         <f t="shared" si="1"/>
         <v>0.25641025641025644</v>
       </c>
-      <c r="F24">
-        <f t="shared" si="2"/>
-        <v>1.2820512820512883E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D25">
         <f t="shared" si="0"/>
         <v>2.3000000000000007</v>
@@ -8500,12 +6922,8 @@
         <f t="shared" si="1"/>
         <v>0.25974025974025977</v>
       </c>
-      <c r="F25">
-        <f t="shared" si="2"/>
-        <v>1.2987012987012979E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D26">
         <f t="shared" si="0"/>
         <v>2.4000000000000008</v>
@@ -8514,12 +6932,8 @@
         <f t="shared" si="1"/>
         <v>0.26315789473684209</v>
       </c>
-      <c r="F26">
-        <f t="shared" si="2"/>
-        <v>1.3157894736841928E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D27">
         <f t="shared" si="0"/>
         <v>2.5000000000000009</v>
@@ -8528,12 +6942,8 @@
         <f t="shared" si="1"/>
         <v>0.26666666666666672</v>
       </c>
-      <c r="F27">
-        <f t="shared" si="2"/>
-        <v>1.3333333333333586E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D28">
         <f t="shared" si="0"/>
         <v>2.600000000000001</v>
@@ -8542,12 +6952,8 @@
         <f t="shared" si="1"/>
         <v>0.27027027027027034</v>
       </c>
-      <c r="F28">
-        <f t="shared" si="2"/>
-        <v>1.351351351351358E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D29">
         <f t="shared" si="0"/>
         <v>2.7000000000000011</v>
@@ -8556,12 +6962,8 @@
         <f t="shared" si="1"/>
         <v>0.27397260273972607</v>
       </c>
-      <c r="F29">
-        <f t="shared" si="2"/>
-        <v>1.3698630136986186E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D30">
         <f t="shared" si="0"/>
         <v>2.8000000000000012</v>
@@ -8570,12 +6972,8 @@
         <f t="shared" si="1"/>
         <v>0.27777777777777779</v>
       </c>
-      <c r="F30">
-        <f t="shared" si="2"/>
-        <v>1.3888888888888784E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D31">
         <f t="shared" si="0"/>
         <v>2.9000000000000012</v>
@@ -8584,12 +6982,8 @@
         <f t="shared" si="1"/>
         <v>0.28169014084507049</v>
       </c>
-      <c r="F31">
-        <f t="shared" si="2"/>
-        <v>1.4084507042253724E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D32">
         <f t="shared" si="0"/>
         <v>3.0000000000000013</v>
@@ -8598,12 +6992,8 @@
         <f t="shared" si="1"/>
         <v>0.28571428571428581</v>
       </c>
-      <c r="F32">
-        <f t="shared" si="2"/>
-        <v>1.4285714285714375E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D33">
         <f t="shared" si="0"/>
         <v>3.1000000000000014</v>
@@ -8612,12 +7002,8 @@
         <f t="shared" si="1"/>
         <v>0.28985507246376818</v>
       </c>
-      <c r="F33">
-        <f t="shared" si="2"/>
-        <v>1.4492753623188298E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D34">
         <f t="shared" si="0"/>
         <v>3.2000000000000015</v>
@@ -8626,12 +7012,8 @@
         <f t="shared" si="1"/>
         <v>0.29411764705882359</v>
       </c>
-      <c r="F34">
-        <f t="shared" si="2"/>
-        <v>1.4705882352941171E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D35">
         <f t="shared" si="0"/>
         <v>3.3000000000000016</v>
@@ -8640,12 +7022,8 @@
         <f t="shared" si="1"/>
         <v>0.29850746268656725</v>
       </c>
-      <c r="F35">
-        <f t="shared" si="2"/>
-        <v>1.492537313432842E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D36">
         <f t="shared" si="0"/>
         <v>3.4000000000000017</v>
@@ -8654,12 +7032,8 @@
         <f t="shared" si="1"/>
         <v>0.30303030303030315</v>
       </c>
-      <c r="F36">
-        <f t="shared" si="2"/>
-        <v>1.5151515151515265E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D37">
         <f t="shared" si="0"/>
         <v>3.5000000000000018</v>
@@ -8668,12 +7042,8 @@
         <f t="shared" si="1"/>
         <v>0.30769230769230776</v>
       </c>
-      <c r="F37">
-        <f t="shared" si="2"/>
-        <v>1.5384615384615224E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D38">
         <f t="shared" si="0"/>
         <v>3.6000000000000019</v>
@@ -8682,12 +7052,8 @@
         <f t="shared" si="1"/>
         <v>0.31250000000000006</v>
       </c>
-      <c r="F38">
-        <f t="shared" si="2"/>
-        <v>1.5624999999999941E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D39">
         <f t="shared" si="0"/>
         <v>3.700000000000002</v>
@@ -8696,12 +7062,8 @@
         <f t="shared" si="1"/>
         <v>0.31746031746031755</v>
       </c>
-      <c r="F39">
-        <f t="shared" si="2"/>
-        <v>1.587301587301599E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D40">
         <f t="shared" si="0"/>
         <v>3.800000000000002</v>
@@ -8710,12 +7072,8 @@
         <f t="shared" si="1"/>
         <v>0.32258064516129042</v>
       </c>
-      <c r="F40">
-        <f t="shared" si="2"/>
-        <v>1.612903225806454E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D41">
         <f t="shared" si="0"/>
         <v>3.9000000000000021</v>
@@ -8724,12 +7082,8 @@
         <f t="shared" si="1"/>
         <v>0.32786885245901654</v>
       </c>
-      <c r="F41">
-        <f t="shared" si="2"/>
-        <v>1.6393442622950938E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D42">
         <f t="shared" si="0"/>
         <v>4.0000000000000018</v>
@@ -8738,12 +7092,8 @@
         <f t="shared" si="1"/>
         <v>0.33333333333333343</v>
       </c>
-      <c r="F42">
-        <f t="shared" si="2"/>
-        <v>1.666666666666651E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D43">
         <f t="shared" si="0"/>
         <v>4.1000000000000014</v>
@@ -8752,12 +7102,8 @@
         <f t="shared" si="1"/>
         <v>0.33898305084745772</v>
       </c>
-      <c r="F43">
-        <f t="shared" si="2"/>
-        <v>1.6949152542372888E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D44">
         <f t="shared" si="0"/>
         <v>4.2000000000000011</v>
@@ -8766,12 +7112,8 @@
         <f t="shared" si="1"/>
         <v>0.34482758620689663</v>
       </c>
-      <c r="F44">
-        <f t="shared" si="2"/>
-        <v>1.7241379310344772E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D45">
         <f t="shared" si="0"/>
         <v>4.3000000000000007</v>
@@ -8780,12 +7122,8 @@
         <f t="shared" si="1"/>
         <v>0.35087719298245618</v>
       </c>
-      <c r="F45">
-        <f t="shared" si="2"/>
-        <v>1.7543859649122681E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D46">
         <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
@@ -8794,12 +7132,8 @@
         <f t="shared" si="1"/>
         <v>0.35714285714285715</v>
       </c>
-      <c r="F46">
-        <f t="shared" si="2"/>
-        <v>1.7857142857142776E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D47">
         <f t="shared" si="0"/>
         <v>4.5</v>
@@ -8808,12 +7142,8 @@
         <f t="shared" si="1"/>
         <v>0.36363636363636365</v>
       </c>
-      <c r="F47">
-        <f t="shared" si="2"/>
-        <v>1.8181818181818188E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D48">
         <f t="shared" si="0"/>
         <v>4.5999999999999996</v>
@@ -8822,12 +7152,8 @@
         <f t="shared" si="1"/>
         <v>0.37037037037037035</v>
       </c>
-      <c r="F48">
-        <f t="shared" si="2"/>
-        <v>1.8518518518518434E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D49">
         <f t="shared" si="0"/>
         <v>4.6999999999999993</v>
@@ -8836,12 +7162,8 @@
         <f t="shared" si="1"/>
         <v>0.37735849056603771</v>
       </c>
-      <c r="F49">
-        <f t="shared" si="2"/>
-        <v>1.8867924528301869E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D50">
         <f t="shared" si="0"/>
         <v>4.7999999999999989</v>
@@ -8850,12 +7172,8 @@
         <f t="shared" si="1"/>
         <v>0.38461538461538453</v>
       </c>
-      <c r="F50">
-        <f t="shared" si="2"/>
-        <v>1.9230769230769069E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D51">
         <f t="shared" si="0"/>
         <v>4.8999999999999986</v>
@@ -8864,12 +7182,8 @@
         <f t="shared" si="1"/>
         <v>0.39215686274509792</v>
       </c>
-      <c r="F51">
-        <f t="shared" si="2"/>
-        <v>1.9607843137254836E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D52">
         <f t="shared" si="0"/>
         <v>4.9999999999999982</v>
@@ -8878,12 +7192,8 @@
         <f t="shared" si="1"/>
         <v>0.39999999999999986</v>
       </c>
-      <c r="F52">
-        <f t="shared" si="2"/>
-        <v>1.9999999999999934E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D53">
         <f t="shared" si="0"/>
         <v>5.0999999999999979</v>
@@ -8892,12 +7202,8 @@
         <f t="shared" si="1"/>
         <v>0.40816326530612229</v>
       </c>
-      <c r="F53">
-        <f t="shared" si="2"/>
-        <v>2.0408163265306097E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D54">
         <f t="shared" si="0"/>
         <v>5.1999999999999975</v>
@@ -8906,12 +7212,8 @@
         <f t="shared" si="1"/>
         <v>0.41666666666666646</v>
       </c>
-      <c r="F54">
-        <f t="shared" si="2"/>
-        <v>2.0833333333333228E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D55">
         <f t="shared" si="0"/>
         <v>5.2999999999999972</v>
@@ -8920,12 +7222,8 @@
         <f t="shared" si="1"/>
         <v>0.42553191489361675</v>
       </c>
-      <c r="F55">
-        <f t="shared" si="2"/>
-        <v>2.1276595744680691E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D56">
         <f t="shared" si="0"/>
         <v>5.3999999999999968</v>
@@ -8934,12 +7232,8 @@
         <f t="shared" si="1"/>
         <v>0.43478260869565188</v>
       </c>
-      <c r="F56">
-        <f t="shared" si="2"/>
-        <v>2.1739130434782587E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D57">
         <f t="shared" si="0"/>
         <v>5.4999999999999964</v>
@@ -8948,12 +7242,8 @@
         <f t="shared" si="1"/>
         <v>0.44444444444444409</v>
       </c>
-      <c r="F57">
-        <f t="shared" si="2"/>
-        <v>2.2222222222222081E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D58">
         <f t="shared" si="0"/>
         <v>5.5999999999999961</v>
@@ -8962,12 +7252,8 @@
         <f t="shared" si="1"/>
         <v>0.45454545454545414</v>
       </c>
-      <c r="F58">
-        <f t="shared" si="2"/>
-        <v>2.2727272727272641E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D59">
         <f t="shared" si="0"/>
         <v>5.6999999999999957</v>
@@ -8976,12 +7262,8 @@
         <f t="shared" si="1"/>
         <v>0.46511627906976699</v>
       </c>
-      <c r="F59">
-        <f t="shared" si="2"/>
-        <v>2.3255813953488289E-2</v>
-      </c>
-    </row>
-    <row r="60" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D60">
         <f t="shared" si="0"/>
         <v>5.7999999999999954</v>
@@ -8990,12 +7272,8 @@
         <f t="shared" si="1"/>
         <v>0.47619047619047566</v>
       </c>
-      <c r="F60">
-        <f t="shared" si="2"/>
-        <v>2.3809523809523669E-2</v>
-      </c>
-    </row>
-    <row r="61" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D61">
         <f t="shared" si="0"/>
         <v>5.899999999999995</v>
@@ -9004,12 +7282,8 @@
         <f t="shared" si="1"/>
         <v>0.48780487804877992</v>
       </c>
-      <c r="F61">
-        <f t="shared" si="2"/>
-        <v>2.4390243902438966E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D62">
         <f t="shared" si="0"/>
         <v>5.9999999999999947</v>
@@ -9018,12 +7292,8 @@
         <f t="shared" si="1"/>
         <v>0.49999999999999933</v>
       </c>
-      <c r="F62">
-        <f t="shared" si="2"/>
-        <v>2.4999999999999824E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D63">
         <f t="shared" si="0"/>
         <v>6.0999999999999943</v>
@@ -9032,12 +7302,8 @@
         <f t="shared" si="1"/>
         <v>0.51282051282051211</v>
       </c>
-      <c r="F63">
-        <f t="shared" si="2"/>
-        <v>2.5641025641025585E-2</v>
-      </c>
-    </row>
-    <row r="64" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D64">
         <f t="shared" si="0"/>
         <v>6.199999999999994</v>
@@ -9046,12 +7312,8 @@
         <f t="shared" si="1"/>
         <v>0.5263157894736834</v>
       </c>
-      <c r="F64">
-        <f t="shared" si="2"/>
-        <v>2.6315789473684063E-2</v>
-      </c>
-    </row>
-    <row r="65" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D65">
         <f t="shared" si="0"/>
         <v>6.2999999999999936</v>
@@ -9060,12 +7322,8 @@
         <f t="shared" si="1"/>
         <v>0.54054054054053957</v>
       </c>
-      <c r="F65">
-        <f t="shared" si="2"/>
-        <v>2.7027027027026758E-2</v>
-      </c>
-    </row>
-    <row r="66" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D66">
         <f t="shared" si="0"/>
         <v>6.3999999999999932</v>
@@ -9074,499 +7332,355 @@
         <f t="shared" si="1"/>
         <v>0.55555555555555447</v>
       </c>
-      <c r="F66">
-        <f t="shared" si="2"/>
-        <v>2.7777777777777613E-2</v>
-      </c>
-    </row>
-    <row r="67" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D67">
         <f t="shared" si="0"/>
         <v>6.4999999999999929</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E101" si="3">$B$4/(D67-$B$5)</f>
+        <f t="shared" ref="E67:E101" si="2">$B$4/(D67-$B$5)</f>
         <v>0.57142857142857029</v>
       </c>
-      <c r="F67">
-        <f t="shared" si="2"/>
-        <v>2.8571428571428525E-2</v>
-      </c>
-    </row>
-    <row r="68" spans="4:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D68">
-        <f t="shared" ref="D68:D101" si="4">($B$2-$B$1)/100+D67</f>
+        <f t="shared" ref="D68:D101" si="3">($B$2-$B$1)/100+D67</f>
         <v>6.5999999999999925</v>
       </c>
       <c r="E68">
+        <f t="shared" si="2"/>
+        <v>0.58823529411764575</v>
+      </c>
+    </row>
+    <row r="69" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D69">
         <f t="shared" si="3"/>
-        <v>0.58823529411764575</v>
-      </c>
-      <c r="F68">
-        <f t="shared" ref="F68:F101" si="5">(E68-E67)/E67</f>
-        <v>2.9411764705882113E-2</v>
-      </c>
-    </row>
-    <row r="69" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D69">
-        <f t="shared" si="4"/>
         <v>6.6999999999999922</v>
       </c>
       <c r="E69">
+        <f t="shared" si="2"/>
+        <v>0.60606060606060463</v>
+      </c>
+    </row>
+    <row r="70" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D70">
         <f t="shared" si="3"/>
-        <v>0.60606060606060463</v>
-      </c>
-      <c r="F69">
-        <f t="shared" si="5"/>
-        <v>3.0303030303030176E-2</v>
-      </c>
-    </row>
-    <row r="70" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D70">
-        <f t="shared" si="4"/>
         <v>6.7999999999999918</v>
       </c>
       <c r="E70">
+        <f t="shared" si="2"/>
+        <v>0.62499999999999845</v>
+      </c>
+    </row>
+    <row r="71" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D71">
         <f t="shared" si="3"/>
-        <v>0.62499999999999845</v>
-      </c>
-      <c r="F70">
-        <f t="shared" si="5"/>
-        <v>3.1249999999999861E-2</v>
-      </c>
-    </row>
-    <row r="71" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D71">
-        <f t="shared" si="4"/>
         <v>6.8999999999999915</v>
       </c>
       <c r="E71">
+        <f t="shared" si="2"/>
+        <v>0.64516129032257885</v>
+      </c>
+    </row>
+    <row r="72" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D72">
         <f t="shared" si="3"/>
-        <v>0.64516129032257885</v>
-      </c>
-      <c r="F71">
-        <f t="shared" si="5"/>
-        <v>3.2258064516128726E-2</v>
-      </c>
-    </row>
-    <row r="72" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D72">
-        <f t="shared" si="4"/>
         <v>6.9999999999999911</v>
       </c>
       <c r="E72">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666474</v>
+      </c>
+    </row>
+    <row r="73" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D73">
         <f t="shared" si="3"/>
-        <v>0.66666666666666474</v>
-      </c>
-      <c r="F72">
-        <f t="shared" si="5"/>
-        <v>3.3333333333333222E-2</v>
-      </c>
-    </row>
-    <row r="73" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D73">
-        <f t="shared" si="4"/>
         <v>7.0999999999999908</v>
       </c>
       <c r="E73">
+        <f t="shared" si="2"/>
+        <v>0.68965517241379093</v>
+      </c>
+    </row>
+    <row r="74" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D74">
         <f t="shared" si="3"/>
-        <v>0.68965517241379093</v>
-      </c>
-      <c r="F73">
-        <f t="shared" si="5"/>
-        <v>3.4482758620689377E-2</v>
-      </c>
-    </row>
-    <row r="74" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D74">
-        <f t="shared" si="4"/>
         <v>7.1999999999999904</v>
       </c>
       <c r="E74">
+        <f t="shared" si="2"/>
+        <v>0.71428571428571186</v>
+      </c>
+    </row>
+    <row r="75" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D75">
         <f t="shared" si="3"/>
-        <v>0.71428571428571186</v>
-      </c>
-      <c r="F74">
-        <f t="shared" si="5"/>
-        <v>3.5714285714285463E-2</v>
-      </c>
-    </row>
-    <row r="75" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D75">
-        <f t="shared" si="4"/>
         <v>7.2999999999999901</v>
       </c>
       <c r="E75">
+        <f t="shared" si="2"/>
+        <v>0.74074074074073804</v>
+      </c>
+    </row>
+    <row r="76" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D76">
         <f t="shared" si="3"/>
-        <v>0.74074074074073804</v>
-      </c>
-      <c r="F75">
-        <f t="shared" si="5"/>
-        <v>3.7037037037036771E-2</v>
-      </c>
-    </row>
-    <row r="76" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D76">
-        <f t="shared" si="4"/>
         <v>7.3999999999999897</v>
       </c>
       <c r="E76">
+        <f t="shared" si="2"/>
+        <v>0.76923076923076616</v>
+      </c>
+    </row>
+    <row r="77" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D77">
         <f t="shared" si="3"/>
-        <v>0.76923076923076616</v>
-      </c>
-      <c r="F76">
-        <f t="shared" si="5"/>
-        <v>3.8461538461538117E-2</v>
-      </c>
-    </row>
-    <row r="77" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D77">
-        <f t="shared" si="4"/>
         <v>7.4999999999999893</v>
       </c>
       <c r="E77">
+        <f t="shared" si="2"/>
+        <v>0.7999999999999966</v>
+      </c>
+    </row>
+    <row r="78" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D78">
         <f t="shared" si="3"/>
-        <v>0.7999999999999966</v>
-      </c>
-      <c r="F77">
-        <f t="shared" si="5"/>
-        <v>3.999999999999973E-2</v>
-      </c>
-    </row>
-    <row r="78" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D78">
-        <f t="shared" si="4"/>
         <v>7.599999999999989</v>
       </c>
       <c r="E78">
+        <f t="shared" si="2"/>
+        <v>0.83333333333332948</v>
+      </c>
+    </row>
+    <row r="79" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D79">
         <f t="shared" si="3"/>
-        <v>0.83333333333332948</v>
-      </c>
-      <c r="F78">
-        <f t="shared" si="5"/>
-        <v>4.1666666666666276E-2</v>
-      </c>
-    </row>
-    <row r="79" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D79">
-        <f t="shared" si="4"/>
         <v>7.6999999999999886</v>
       </c>
       <c r="E79">
+        <f t="shared" si="2"/>
+        <v>0.8695652173913001</v>
+      </c>
+    </row>
+    <row r="80" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D80">
         <f t="shared" si="3"/>
-        <v>0.8695652173913001</v>
-      </c>
-      <c r="F79">
-        <f t="shared" si="5"/>
-        <v>4.3478260869564946E-2</v>
-      </c>
-    </row>
-    <row r="80" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D80">
-        <f t="shared" si="4"/>
         <v>7.7999999999999883</v>
       </c>
       <c r="E80">
+        <f t="shared" si="2"/>
+        <v>0.90909090909090429</v>
+      </c>
+    </row>
+    <row r="81" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D81">
         <f t="shared" si="3"/>
-        <v>0.90909090909090429</v>
-      </c>
-      <c r="F80">
-        <f t="shared" si="5"/>
-        <v>4.5454545454545033E-2</v>
-      </c>
-    </row>
-    <row r="81" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D81">
-        <f t="shared" si="4"/>
         <v>7.8999999999999879</v>
       </c>
       <c r="E81">
+        <f t="shared" si="2"/>
+        <v>0.95238095238094689</v>
+      </c>
+    </row>
+    <row r="82" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D82">
         <f t="shared" si="3"/>
-        <v>0.95238095238094689</v>
-      </c>
-      <c r="F81">
-        <f t="shared" si="5"/>
-        <v>4.761904761904711E-2</v>
-      </c>
-    </row>
-    <row r="82" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D82">
-        <f t="shared" si="4"/>
         <v>7.9999999999999876</v>
       </c>
       <c r="E82">
+        <f t="shared" si="2"/>
+        <v>0.99999999999999378</v>
+      </c>
+    </row>
+    <row r="83" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D83">
         <f t="shared" si="3"/>
-        <v>0.99999999999999378</v>
-      </c>
-      <c r="F82">
-        <f t="shared" si="5"/>
-        <v>4.9999999999999531E-2</v>
-      </c>
-    </row>
-    <row r="83" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D83">
-        <f t="shared" si="4"/>
         <v>8.0999999999999872</v>
       </c>
       <c r="E83">
+        <f t="shared" si="2"/>
+        <v>1.0526315789473613</v>
+      </c>
+    </row>
+    <row r="84" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D84">
         <f t="shared" si="3"/>
-        <v>1.0526315789473613</v>
-      </c>
-      <c r="F83">
-        <f t="shared" si="5"/>
-        <v>5.2631578947367801E-2</v>
-      </c>
-    </row>
-    <row r="84" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D84">
-        <f t="shared" si="4"/>
         <v>8.1999999999999869</v>
       </c>
       <c r="E84">
+        <f t="shared" si="2"/>
+        <v>1.1111111111111029</v>
+      </c>
+    </row>
+    <row r="85" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D85">
         <f t="shared" si="3"/>
-        <v>1.1111111111111029</v>
-      </c>
-      <c r="F84">
-        <f t="shared" si="5"/>
-        <v>5.5555555555554983E-2</v>
-      </c>
-    </row>
-    <row r="85" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D85">
-        <f t="shared" si="4"/>
         <v>8.2999999999999865</v>
       </c>
       <c r="E85">
+        <f t="shared" si="2"/>
+        <v>1.1764705882352848</v>
+      </c>
+    </row>
+    <row r="86" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D86">
         <f t="shared" si="3"/>
-        <v>1.1764705882352848</v>
-      </c>
-      <c r="F85">
-        <f t="shared" si="5"/>
-        <v>5.8823529411764129E-2</v>
-      </c>
-    </row>
-    <row r="86" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D86">
-        <f t="shared" si="4"/>
         <v>8.3999999999999861</v>
       </c>
       <c r="E86">
+        <f t="shared" si="2"/>
+        <v>1.2499999999999891</v>
+      </c>
+    </row>
+    <row r="87" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D87">
         <f t="shared" si="3"/>
-        <v>1.2499999999999891</v>
-      </c>
-      <c r="F86">
-        <f t="shared" si="5"/>
-        <v>6.249999999999914E-2</v>
-      </c>
-    </row>
-    <row r="87" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D87">
-        <f t="shared" si="4"/>
         <v>8.4999999999999858</v>
       </c>
       <c r="E87">
+        <f t="shared" si="2"/>
+        <v>1.3333333333333206</v>
+      </c>
+    </row>
+    <row r="88" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D88">
         <f t="shared" si="3"/>
-        <v>1.3333333333333206</v>
-      </c>
-      <c r="F87">
-        <f t="shared" si="5"/>
-        <v>6.6666666666665764E-2</v>
-      </c>
-    </row>
-    <row r="88" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D88">
-        <f t="shared" si="4"/>
         <v>8.5999999999999854</v>
       </c>
       <c r="E88">
+        <f t="shared" si="2"/>
+        <v>1.4285714285714137</v>
+      </c>
+    </row>
+    <row r="89" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D89">
         <f t="shared" si="3"/>
-        <v>1.4285714285714137</v>
-      </c>
-      <c r="F88">
-        <f t="shared" si="5"/>
-        <v>7.1428571428570523E-2</v>
-      </c>
-    </row>
-    <row r="89" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D89">
-        <f t="shared" si="4"/>
         <v>8.6999999999999851</v>
       </c>
       <c r="E89">
+        <f t="shared" si="2"/>
+        <v>1.5384615384615208</v>
+      </c>
+    </row>
+    <row r="90" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D90">
         <f t="shared" si="3"/>
-        <v>1.5384615384615208</v>
-      </c>
-      <c r="F89">
-        <f t="shared" si="5"/>
-        <v>7.6923076923075734E-2</v>
-      </c>
-    </row>
-    <row r="90" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D90">
-        <f t="shared" si="4"/>
         <v>8.7999999999999847</v>
       </c>
       <c r="E90">
+        <f t="shared" si="2"/>
+        <v>1.6666666666666454</v>
+      </c>
+    </row>
+    <row r="91" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D91">
         <f t="shared" si="3"/>
-        <v>1.6666666666666454</v>
-      </c>
-      <c r="F90">
-        <f t="shared" si="5"/>
-        <v>8.3333333333331969E-2</v>
-      </c>
-    </row>
-    <row r="91" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D91">
-        <f t="shared" si="4"/>
         <v>8.8999999999999844</v>
       </c>
       <c r="E91">
+        <f t="shared" si="2"/>
+        <v>1.8181818181817924</v>
+      </c>
+    </row>
+    <row r="92" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D92">
         <f t="shared" si="3"/>
-        <v>1.8181818181817924</v>
-      </c>
-      <c r="F91">
-        <f t="shared" si="5"/>
-        <v>9.0909090909089316E-2</v>
-      </c>
-    </row>
-    <row r="92" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D92">
-        <f t="shared" si="4"/>
         <v>8.999999999999984</v>
       </c>
       <c r="E92">
+        <f t="shared" si="2"/>
+        <v>1.999999999999968</v>
+      </c>
+    </row>
+    <row r="93" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D93">
         <f t="shared" si="3"/>
-        <v>1.999999999999968</v>
-      </c>
-      <c r="F92">
-        <f t="shared" si="5"/>
-        <v>9.9999999999998035E-2</v>
-      </c>
-    </row>
-    <row r="93" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D93">
-        <f t="shared" si="4"/>
         <v>9.0999999999999837</v>
       </c>
       <c r="E93">
+        <f t="shared" si="2"/>
+        <v>2.2222222222221819</v>
+      </c>
+    </row>
+    <row r="94" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D94">
         <f t="shared" si="3"/>
-        <v>2.2222222222221819</v>
-      </c>
-      <c r="F93">
-        <f t="shared" si="5"/>
-        <v>0.11111111111110872</v>
-      </c>
-    </row>
-    <row r="94" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D94">
-        <f t="shared" si="4"/>
         <v>9.1999999999999833</v>
       </c>
       <c r="E94">
+        <f t="shared" si="2"/>
+        <v>2.499999999999948</v>
+      </c>
+    </row>
+    <row r="95" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D95">
         <f t="shared" si="3"/>
-        <v>2.499999999999948</v>
-      </c>
-      <c r="F94">
-        <f t="shared" si="5"/>
-        <v>0.12499999999999703</v>
-      </c>
-    </row>
-    <row r="95" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D95">
-        <f t="shared" si="4"/>
         <v>9.2999999999999829</v>
       </c>
       <c r="E95">
+        <f t="shared" si="2"/>
+        <v>2.8571428571427875</v>
+      </c>
+    </row>
+    <row r="96" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D96">
         <f t="shared" si="3"/>
-        <v>2.8571428571427875</v>
-      </c>
-      <c r="F95">
-        <f t="shared" si="5"/>
-        <v>0.14285714285713874</v>
-      </c>
-    </row>
-    <row r="96" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D96">
-        <f t="shared" si="4"/>
         <v>9.3999999999999826</v>
       </c>
       <c r="E96">
+        <f t="shared" si="2"/>
+        <v>3.3333333333332367</v>
+      </c>
+    </row>
+    <row r="97" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D97">
         <f t="shared" si="3"/>
-        <v>3.3333333333332367</v>
-      </c>
-      <c r="F96">
-        <f t="shared" si="5"/>
-        <v>0.16666666666666127</v>
-      </c>
-    </row>
-    <row r="97" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D97">
-        <f t="shared" si="4"/>
         <v>9.4999999999999822</v>
       </c>
       <c r="E97">
+        <f t="shared" si="2"/>
+        <v>3.9999999999998579</v>
+      </c>
+    </row>
+    <row r="98" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D98">
         <f t="shared" si="3"/>
-        <v>3.9999999999998579</v>
-      </c>
-      <c r="F97">
-        <f t="shared" si="5"/>
-        <v>0.19999999999999216</v>
-      </c>
-    </row>
-    <row r="98" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D98">
-        <f t="shared" si="4"/>
         <v>9.5999999999999819</v>
       </c>
       <c r="E98">
+        <f t="shared" si="2"/>
+        <v>4.9999999999997735</v>
+      </c>
+    </row>
+    <row r="99" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D99">
         <f t="shared" si="3"/>
-        <v>4.9999999999997735</v>
-      </c>
-      <c r="F98">
-        <f t="shared" si="5"/>
-        <v>0.24999999999998779</v>
-      </c>
-    </row>
-    <row r="99" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D99">
-        <f t="shared" si="4"/>
         <v>9.6999999999999815</v>
       </c>
       <c r="E99">
+        <f t="shared" si="2"/>
+        <v>6.6666666666662557</v>
+      </c>
+    </row>
+    <row r="100" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D100">
         <f t="shared" si="3"/>
-        <v>6.6666666666662557</v>
-      </c>
-      <c r="F99">
-        <f t="shared" si="5"/>
-        <v>0.33333333333331155</v>
-      </c>
-    </row>
-    <row r="100" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D100">
-        <f t="shared" si="4"/>
         <v>9.7999999999999812</v>
       </c>
       <c r="E100">
+        <f t="shared" si="2"/>
+        <v>9.9999999999990585</v>
+      </c>
+    </row>
+    <row r="101" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D101">
         <f t="shared" si="3"/>
-        <v>9.9999999999990585</v>
-      </c>
-      <c r="F100">
-        <f t="shared" si="5"/>
-        <v>0.49999999999995126</v>
-      </c>
-    </row>
-    <row r="101" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D101">
-        <f t="shared" si="4"/>
         <v>9.8999999999999808</v>
       </c>
       <c r="E101">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>19.999999999996163</v>
-      </c>
-      <c r="F101">
-        <f t="shared" si="5"/>
-        <v>0.9999999999998046</v>
       </c>
     </row>
   </sheetData>

</xml_diff>